<commit_message>
ScoreHunter Supports the Cer in the [M+H]+
Comments:
Bugs:
- Few bugs where found. Currently run the program with single spectra identification (for all the different lipid groups). Need to check in bigger range.

Addition:
- Can calculate and return the Rank score for the ceramides identification spectra.
- All the classes supported with more dynamic code, same concept as lipidComposer.py

Feature:
- There a few quenstion and points that are need clarification or better solution.
- Identify any possible bugs for the bigger range
- Start making changes so will produce the figures for all the different lipid classes.
- Start apply different filters to avoid false positive identifications for ceramides.
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/1-FA_Whitelist_cER.xlsx
+++ b/ConfigurationFiles/1-FA_Whitelist_cER.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8477"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="78">
   <si>
     <t>FattyAcid</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>FA25:2</t>
+  </si>
+  <si>
+    <t>PL</t>
   </si>
 </sst>
 </file>
@@ -567,18 +570,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="K73" sqref="K73"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39:H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" customWidth="1"/>
+    <col min="1" max="1" width="11.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -592,28 +595,31 @@
         <v>60</v>
       </c>
       <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>69</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>70</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>71</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -626,20 +632,11 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -652,20 +649,11 @@
       <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -678,20 +666,11 @@
       <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -704,20 +683,11 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -730,20 +700,11 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -756,20 +717,11 @@
       <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -782,20 +734,11 @@
       <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -808,20 +751,11 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -834,20 +768,11 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -860,20 +785,11 @@
       <c r="D11" t="s">
         <v>18</v>
       </c>
-      <c r="E11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -886,29 +802,11 @@
       <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" t="s">
-        <v>18</v>
-      </c>
       <c r="I12" t="s">
         <v>18</v>
       </c>
-      <c r="J12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -921,29 +819,11 @@
       <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" t="s">
-        <v>18</v>
-      </c>
       <c r="I13" t="s">
         <v>18</v>
       </c>
-      <c r="J13" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -956,29 +836,11 @@
       <c r="D14" t="s">
         <v>18</v>
       </c>
-      <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" t="s">
-        <v>18</v>
-      </c>
       <c r="I14" t="s">
         <v>18</v>
       </c>
-      <c r="J14" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -991,29 +853,11 @@
       <c r="D15" t="s">
         <v>18</v>
       </c>
-      <c r="E15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" t="s">
-        <v>18</v>
-      </c>
       <c r="I15" t="s">
         <v>18</v>
       </c>
-      <c r="J15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1026,29 +870,11 @@
       <c r="D16" t="s">
         <v>18</v>
       </c>
-      <c r="E16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" t="s">
-        <v>18</v>
-      </c>
       <c r="I16" t="s">
         <v>18</v>
       </c>
-      <c r="J16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1061,29 +887,11 @@
       <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="E17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" t="s">
-        <v>18</v>
-      </c>
       <c r="I17" t="s">
         <v>18</v>
       </c>
-      <c r="J17" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1096,29 +904,11 @@
       <c r="D18" t="s">
         <v>18</v>
       </c>
-      <c r="E18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" t="s">
-        <v>18</v>
-      </c>
       <c r="I18" t="s">
         <v>18</v>
       </c>
-      <c r="J18" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1131,29 +921,11 @@
       <c r="D19" t="s">
         <v>18</v>
       </c>
-      <c r="E19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" t="s">
-        <v>18</v>
-      </c>
       <c r="I19" t="s">
         <v>18</v>
       </c>
-      <c r="J19" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1166,29 +938,11 @@
       <c r="D20" t="s">
         <v>18</v>
       </c>
-      <c r="E20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" t="s">
-        <v>18</v>
-      </c>
       <c r="I20" t="s">
         <v>18</v>
       </c>
-      <c r="J20" t="s">
-        <v>18</v>
-      </c>
-      <c r="K20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1204,12 +958,6 @@
       <c r="E21" t="s">
         <v>18</v>
       </c>
-      <c r="F21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" t="s">
-        <v>18</v>
-      </c>
       <c r="H21" t="s">
         <v>18</v>
       </c>
@@ -1222,8 +970,11 @@
       <c r="K21" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1239,12 +990,6 @@
       <c r="E22" t="s">
         <v>18</v>
       </c>
-      <c r="F22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" t="s">
-        <v>18</v>
-      </c>
       <c r="H22" t="s">
         <v>18</v>
       </c>
@@ -1257,8 +1002,11 @@
       <c r="K22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1271,18 +1019,6 @@
       <c r="D23" t="s">
         <v>18</v>
       </c>
-      <c r="E23" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" t="s">
-        <v>18</v>
-      </c>
       <c r="I23" t="s">
         <v>18</v>
       </c>
@@ -1292,8 +1028,11 @@
       <c r="K23" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1306,29 +1045,11 @@
       <c r="D24" t="s">
         <v>18</v>
       </c>
-      <c r="E24" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" t="s">
-        <v>18</v>
-      </c>
       <c r="I24" t="s">
         <v>18</v>
       </c>
-      <c r="J24" t="s">
-        <v>18</v>
-      </c>
-      <c r="K24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1341,29 +1062,11 @@
       <c r="D25" t="s">
         <v>18</v>
       </c>
-      <c r="E25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" t="s">
-        <v>18</v>
-      </c>
       <c r="I25" t="s">
         <v>18</v>
       </c>
-      <c r="J25" t="s">
-        <v>18</v>
-      </c>
-      <c r="K25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1376,29 +1079,11 @@
       <c r="D26" t="s">
         <v>18</v>
       </c>
-      <c r="E26" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" t="s">
-        <v>18</v>
-      </c>
       <c r="I26" t="s">
         <v>18</v>
       </c>
-      <c r="J26" t="s">
-        <v>18</v>
-      </c>
-      <c r="K26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1414,12 +1099,6 @@
       <c r="E27" t="s">
         <v>18</v>
       </c>
-      <c r="F27" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" t="s">
-        <v>18</v>
-      </c>
       <c r="H27" t="s">
         <v>18</v>
       </c>
@@ -1432,8 +1111,11 @@
       <c r="K27" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1449,9 +1131,6 @@
       <c r="E28" t="s">
         <v>18</v>
       </c>
-      <c r="F28" t="s">
-        <v>18</v>
-      </c>
       <c r="G28" t="s">
         <v>18</v>
       </c>
@@ -1467,8 +1146,11 @@
       <c r="K28" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1496,14 +1178,8 @@
       <c r="I29" t="s">
         <v>18</v>
       </c>
-      <c r="J29" t="s">
-        <v>18</v>
-      </c>
-      <c r="K29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1516,20 +1192,14 @@
       <c r="D30" t="s">
         <v>18</v>
       </c>
-      <c r="E30" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" t="s">
-        <v>18</v>
-      </c>
       <c r="G30" t="s">
         <v>18</v>
       </c>
-      <c r="H30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1542,20 +1212,11 @@
       <c r="D31" t="s">
         <v>18</v>
       </c>
-      <c r="E31" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -1568,29 +1229,11 @@
       <c r="D32" t="s">
         <v>18</v>
       </c>
-      <c r="E32" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" t="s">
-        <v>18</v>
-      </c>
       <c r="I32" t="s">
         <v>18</v>
       </c>
-      <c r="J32" t="s">
-        <v>18</v>
-      </c>
-      <c r="K32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -1603,29 +1246,11 @@
       <c r="D33" t="s">
         <v>18</v>
       </c>
-      <c r="E33" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G33" t="s">
-        <v>18</v>
-      </c>
-      <c r="H33" t="s">
-        <v>18</v>
-      </c>
       <c r="I33" t="s">
         <v>18</v>
       </c>
-      <c r="J33" t="s">
-        <v>18</v>
-      </c>
-      <c r="K33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -1638,29 +1263,11 @@
       <c r="D34" t="s">
         <v>18</v>
       </c>
-      <c r="E34" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" t="s">
-        <v>18</v>
-      </c>
-      <c r="H34" t="s">
-        <v>18</v>
-      </c>
       <c r="I34" t="s">
         <v>18</v>
       </c>
-      <c r="J34" t="s">
-        <v>18</v>
-      </c>
-      <c r="K34" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1676,15 +1283,6 @@
       <c r="E35" t="s">
         <v>18</v>
       </c>
-      <c r="F35" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" t="s">
-        <v>18</v>
-      </c>
-      <c r="H35" t="s">
-        <v>18</v>
-      </c>
       <c r="I35" t="s">
         <v>18</v>
       </c>
@@ -1694,8 +1292,11 @@
       <c r="K35" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -1708,29 +1309,11 @@
       <c r="D36" t="s">
         <v>18</v>
       </c>
-      <c r="E36" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" t="s">
-        <v>18</v>
-      </c>
-      <c r="G36" t="s">
-        <v>18</v>
-      </c>
-      <c r="H36" t="s">
-        <v>18</v>
-      </c>
       <c r="I36" t="s">
         <v>18</v>
       </c>
-      <c r="J36" t="s">
-        <v>18</v>
-      </c>
-      <c r="K36" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1743,29 +1326,11 @@
       <c r="D37" t="s">
         <v>18</v>
       </c>
-      <c r="E37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" t="s">
-        <v>18</v>
-      </c>
-      <c r="G37" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" t="s">
-        <v>18</v>
-      </c>
       <c r="I37" t="s">
         <v>18</v>
       </c>
-      <c r="J37" t="s">
-        <v>18</v>
-      </c>
-      <c r="K37" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1778,20 +1343,11 @@
       <c r="D38" t="s">
         <v>18</v>
       </c>
-      <c r="E38" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H38" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1807,17 +1363,11 @@
       <c r="E39" t="s">
         <v>18</v>
       </c>
-      <c r="F39" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" t="s">
-        <v>18</v>
-      </c>
-      <c r="H39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1830,20 +1380,11 @@
       <c r="D40" t="s">
         <v>18</v>
       </c>
-      <c r="E40" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" t="s">
-        <v>18</v>
-      </c>
-      <c r="H40" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -1856,29 +1397,11 @@
       <c r="D41" t="s">
         <v>18</v>
       </c>
-      <c r="E41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" t="s">
-        <v>18</v>
-      </c>
-      <c r="H41" t="s">
-        <v>18</v>
-      </c>
       <c r="I41" t="s">
         <v>18</v>
       </c>
-      <c r="J41" t="s">
-        <v>18</v>
-      </c>
-      <c r="K41" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -1891,29 +1414,11 @@
       <c r="D42" t="s">
         <v>18</v>
       </c>
-      <c r="E42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F42" t="s">
-        <v>18</v>
-      </c>
-      <c r="G42" t="s">
-        <v>18</v>
-      </c>
-      <c r="H42" t="s">
-        <v>18</v>
-      </c>
       <c r="I42" t="s">
         <v>18</v>
       </c>
-      <c r="J42" t="s">
-        <v>18</v>
-      </c>
-      <c r="K42" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -1926,29 +1431,11 @@
       <c r="D43" t="s">
         <v>18</v>
       </c>
-      <c r="E43" t="s">
-        <v>18</v>
-      </c>
-      <c r="F43" t="s">
-        <v>18</v>
-      </c>
-      <c r="G43" t="s">
-        <v>18</v>
-      </c>
-      <c r="H43" t="s">
-        <v>18</v>
-      </c>
       <c r="I43" t="s">
         <v>18</v>
       </c>
-      <c r="J43" t="s">
-        <v>18</v>
-      </c>
-      <c r="K43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -1961,20 +1448,11 @@
       <c r="D44" t="s">
         <v>18</v>
       </c>
-      <c r="E44" t="s">
-        <v>18</v>
-      </c>
-      <c r="F44" t="s">
-        <v>18</v>
-      </c>
-      <c r="G44" t="s">
-        <v>18</v>
-      </c>
-      <c r="H44" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1987,20 +1465,11 @@
       <c r="D45" t="s">
         <v>18</v>
       </c>
-      <c r="E45" t="s">
-        <v>18</v>
-      </c>
-      <c r="F45" t="s">
-        <v>18</v>
-      </c>
-      <c r="G45" t="s">
-        <v>18</v>
-      </c>
-      <c r="H45" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -2013,20 +1482,11 @@
       <c r="D46" t="s">
         <v>18</v>
       </c>
-      <c r="E46" t="s">
-        <v>18</v>
-      </c>
-      <c r="F46" t="s">
-        <v>18</v>
-      </c>
-      <c r="G46" t="s">
-        <v>18</v>
-      </c>
-      <c r="H46" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I46" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -2039,17 +1499,11 @@
       <c r="D47" t="s">
         <v>18</v>
       </c>
-      <c r="E47" t="s">
-        <v>18</v>
-      </c>
-      <c r="F47" t="s">
-        <v>18</v>
-      </c>
-      <c r="H47" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -2065,63 +1519,33 @@
       <c r="E48" t="s">
         <v>18</v>
       </c>
-      <c r="F48" t="s">
-        <v>18</v>
-      </c>
-      <c r="H48" t="s">
-        <v>18</v>
-      </c>
       <c r="I48" t="s">
         <v>18</v>
       </c>
-      <c r="J48" t="s">
-        <v>18</v>
-      </c>
-      <c r="K48" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>73</v>
       </c>
       <c r="B49" t="s">
         <v>18</v>
       </c>
-      <c r="H49" t="s">
-        <v>18</v>
-      </c>
       <c r="I49" t="s">
         <v>18</v>
       </c>
-      <c r="J49" t="s">
-        <v>18</v>
-      </c>
-      <c r="K49" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>74</v>
       </c>
       <c r="B50" t="s">
         <v>18</v>
       </c>
-      <c r="H50" t="s">
-        <v>18</v>
-      </c>
       <c r="I50" t="s">
         <v>18</v>
       </c>
-      <c r="J50" t="s">
-        <v>18</v>
-      </c>
-      <c r="K50" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>25</v>
       </c>
@@ -2134,26 +1558,11 @@
       <c r="D51" t="s">
         <v>18</v>
       </c>
-      <c r="E51" t="s">
-        <v>18</v>
-      </c>
-      <c r="F51" t="s">
-        <v>18</v>
-      </c>
-      <c r="H51" t="s">
-        <v>18</v>
-      </c>
       <c r="I51" t="s">
         <v>18</v>
       </c>
-      <c r="J51" t="s">
-        <v>18</v>
-      </c>
-      <c r="K51" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -2166,26 +1575,11 @@
       <c r="D52" t="s">
         <v>18</v>
       </c>
-      <c r="E52" t="s">
-        <v>18</v>
-      </c>
-      <c r="F52" t="s">
-        <v>18</v>
-      </c>
-      <c r="H52" t="s">
-        <v>18</v>
-      </c>
       <c r="I52" t="s">
         <v>18</v>
       </c>
-      <c r="J52" t="s">
-        <v>18</v>
-      </c>
-      <c r="K52" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -2198,26 +1592,11 @@
       <c r="D53" t="s">
         <v>18</v>
       </c>
-      <c r="E53" t="s">
-        <v>18</v>
-      </c>
-      <c r="F53" t="s">
-        <v>18</v>
-      </c>
-      <c r="H53" t="s">
-        <v>18</v>
-      </c>
       <c r="I53" t="s">
         <v>18</v>
       </c>
-      <c r="J53" t="s">
-        <v>18</v>
-      </c>
-      <c r="K53" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -2230,17 +1609,11 @@
       <c r="D54" t="s">
         <v>18</v>
       </c>
-      <c r="E54" t="s">
-        <v>18</v>
-      </c>
-      <c r="F54" t="s">
-        <v>18</v>
-      </c>
-      <c r="H54" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I54" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -2253,66 +1626,33 @@
       <c r="D55" t="s">
         <v>18</v>
       </c>
-      <c r="E55" t="s">
-        <v>18</v>
-      </c>
-      <c r="F55" t="s">
-        <v>18</v>
-      </c>
-      <c r="H55" t="s">
-        <v>18</v>
-      </c>
       <c r="I55" t="s">
         <v>18</v>
       </c>
-      <c r="J55" t="s">
-        <v>18</v>
-      </c>
-      <c r="K55" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>75</v>
       </c>
       <c r="B56" t="s">
         <v>18</v>
       </c>
-      <c r="H56" t="s">
-        <v>18</v>
-      </c>
       <c r="I56" t="s">
         <v>18</v>
       </c>
-      <c r="J56" t="s">
-        <v>18</v>
-      </c>
-      <c r="K56" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>76</v>
       </c>
       <c r="B57" t="s">
         <v>18</v>
       </c>
-      <c r="H57" t="s">
-        <v>18</v>
-      </c>
       <c r="I57" t="s">
         <v>18</v>
       </c>
-      <c r="J57" t="s">
-        <v>18</v>
-      </c>
-      <c r="K57" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>26</v>
       </c>
@@ -2325,26 +1665,11 @@
       <c r="D58" t="s">
         <v>18</v>
       </c>
-      <c r="E58" t="s">
-        <v>18</v>
-      </c>
-      <c r="F58" t="s">
-        <v>18</v>
-      </c>
-      <c r="H58" t="s">
-        <v>18</v>
-      </c>
       <c r="I58" t="s">
         <v>18</v>
       </c>
-      <c r="J58" t="s">
-        <v>18</v>
-      </c>
-      <c r="K58" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -2357,26 +1682,11 @@
       <c r="D59" t="s">
         <v>18</v>
       </c>
-      <c r="E59" t="s">
-        <v>18</v>
-      </c>
-      <c r="F59" t="s">
-        <v>18</v>
-      </c>
-      <c r="H59" t="s">
-        <v>18</v>
-      </c>
       <c r="I59" t="s">
         <v>18</v>
       </c>
-      <c r="J59" t="s">
-        <v>18</v>
-      </c>
-      <c r="K59" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -2389,26 +1699,11 @@
       <c r="D60" t="s">
         <v>18</v>
       </c>
-      <c r="E60" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" t="s">
-        <v>18</v>
-      </c>
-      <c r="H60" t="s">
-        <v>18</v>
-      </c>
       <c r="I60" t="s">
         <v>18</v>
       </c>
-      <c r="J60" t="s">
-        <v>18</v>
-      </c>
-      <c r="K60" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -2418,11 +1713,8 @@
       <c r="E61" t="s">
         <v>18</v>
       </c>
-      <c r="F61" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>13</v>
       </c>
@@ -2432,11 +1724,8 @@
       <c r="E62" t="s">
         <v>18</v>
       </c>
-      <c r="F62" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -2446,11 +1735,8 @@
       <c r="E63" t="s">
         <v>18</v>
       </c>
-      <c r="F63" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -2460,11 +1746,8 @@
       <c r="E64" t="s">
         <v>18</v>
       </c>
-      <c r="F64" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -2474,11 +1757,8 @@
       <c r="E65" t="s">
         <v>18</v>
       </c>
-      <c r="F65" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -2486,9 +1766,6 @@
         <v>18</v>
       </c>
       <c r="E66" t="s">
-        <v>18</v>
-      </c>
-      <c r="F66" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>